<commit_message>
Oppdatert excel hack og xlsx-fil
</commit_message>
<xml_diff>
--- a/Data/OPXfinansAGA.xlsx
+++ b/Data/OPXfinansAGA.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gusia\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gusia\Desktop\HACKATHON\ISSSV1337\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{328D4F08-9BCB-4BF5-8F88-1A48EA727759}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C61195CC-051D-40D4-BE97-C077112469D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{FF0D3A43-FCC6-2A45-ABA7-E28E53F8BFCB}"/>
+    <workbookView xWindow="2260" yWindow="1870" windowWidth="14400" windowHeight="7270" xr2:uid="{FF0D3A43-FCC6-2A45-ABA7-E28E53F8BFCB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -599,9 +599,7 @@
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="3">
-        <v>462196</v>
-      </c>
+      <c r="B4" s="3"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">

</xml_diff>